<commit_message>
Sheet Linking - removed START_SESSION things, update your Control.definition! - added main sheet template to tamplates - SessionSheet now links to main file and vice versa - fixed crash when enemy count is zero - added constants for main sheet template
</commit_message>
<xml_diff>
--- a/Templates/Templates.xlsx
+++ b/Templates/Templates.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Metin2 Drop Analyzer\Metin2SpeechToData\bin\Debug\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Metin2DropAnalyzer\Metin2SpeechToData\bin\Debug\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9C19B1-7E56-4CD5-9503-2414A8A3A701}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B687507-ABB4-4387-BCBB-8EE266342188}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Area" sheetId="5" r:id="rId1"/>
-    <sheet name="Enemy" sheetId="2" r:id="rId2"/>
-    <sheet name="Session" sheetId="6" r:id="rId3"/>
+    <sheet name="Main" sheetId="7" r:id="rId1"/>
+    <sheet name="Area" sheetId="5" r:id="rId2"/>
+    <sheet name="Enemy" sheetId="2" r:id="rId3"/>
+    <sheet name="Session" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <r>
       <rPr>
@@ -145,12 +146,27 @@
   <si>
     <t>Item</t>
   </si>
+  <si>
+    <t>Existing sheets</t>
+  </si>
+  <si>
+    <t>Merged Sessions</t>
+  </si>
+  <si>
+    <t>Unmerged Sessions</t>
+  </si>
+  <si>
+    <t>Metin2 siNDiCATE Drop Analyzer/Logger</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,###"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -220,8 +236,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="36"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,8 +311,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEED782"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="46">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -870,13 +899,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -920,21 +1062,77 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -944,74 +1142,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1022,90 +1153,163 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1182,6 +1386,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFEED782"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1490,39 +1697,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D37D157-3B5C-4918-9447-DD7F6F6CF083}">
+  <dimension ref="A1:U25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B2" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="50"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="53"/>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="55"/>
+      <c r="U4" s="56"/>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
+      <c r="U5" s="46"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="D6" s="134" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="136"/>
+      <c r="J6" s="134" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="135"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="136"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="134" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="135"/>
+      <c r="S6" s="136"/>
+      <c r="U6" s="21"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="137"/>
+      <c r="L7" s="137"/>
+      <c r="M7" s="137"/>
+      <c r="P7" s="137"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="137"/>
+      <c r="S7" s="137"/>
+      <c r="U7" s="21"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="U8" s="21"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="U9" s="21"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="U10" s="21"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="U11" s="47"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="U12" s="47"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="U13" s="47"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="U14" s="47"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="U15" s="47"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="U16" s="47"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="47"/>
+      <c r="U17" s="47"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="45"/>
+      <c r="U18" s="47"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="45"/>
+      <c r="U19" s="45"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="45"/>
+      <c r="U20" s="45"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="45"/>
+      <c r="U21" s="45"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="45"/>
+      <c r="U22" s="45"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="45"/>
+      <c r="U23" s="45"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="45"/>
+      <c r="U24" s="45"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U25" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="B2:U4"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="D7:G7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E4C1B2-82A3-4D72-8863-46DE92AE18FA}">
   <dimension ref="B1:AG47"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6:Q6"/>
+    <sheetView topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1"/>
-    <col min="15" max="15" width="30.6640625" customWidth="1"/>
-    <col min="19" max="19" width="30.6640625" customWidth="1"/>
-    <col min="23" max="23" width="30.6640625" customWidth="1"/>
-    <col min="27" max="27" width="30.6640625" customWidth="1"/>
-    <col min="31" max="31" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" customWidth="1"/>
+    <col min="19" max="19" width="30.7109375" customWidth="1"/>
+    <col min="23" max="23" width="30.7109375" customWidth="1"/>
+    <col min="27" max="27" width="30.7109375" customWidth="1"/>
+    <col min="31" max="31" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:33" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="56" t="s">
+    <row r="1" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
       <c r="L2" s="40"/>
       <c r="M2" s="40"/>
       <c r="N2" s="40"/>
@@ -1530,35 +1947,35 @@
       <c r="P2" s="40"/>
       <c r="Q2" s="40"/>
       <c r="R2" s="40"/>
-      <c r="S2" s="60" t="s">
+      <c r="S2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="60"/>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="61"/>
-    </row>
-    <row r="3" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B3" s="58"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+      <c r="AD2" s="61"/>
+      <c r="AE2" s="61"/>
+      <c r="AF2" s="61"/>
+      <c r="AG2" s="62"/>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
       <c r="L3" s="2"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -1566,25 +1983,25 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="44" t="s">
+      <c r="S3" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="44"/>
-      <c r="Z3" s="44"/>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="44"/>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
-      <c r="AG3" s="45"/>
-    </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="65"/>
+    </row>
+    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B4" s="41"/>
       <c r="C4" s="2"/>
       <c r="D4" s="5"/>
@@ -1596,237 +2013,237 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="49" t="s">
+      <c r="M4" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="44" t="s">
+      <c r="S4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="44"/>
-      <c r="X4" s="44"/>
-      <c r="Y4" s="44"/>
-      <c r="Z4" s="44"/>
-      <c r="AA4" s="44"/>
-      <c r="AB4" s="44"/>
-      <c r="AC4" s="44"/>
-      <c r="AD4" s="44"/>
-      <c r="AE4" s="44"/>
-      <c r="AF4" s="44"/>
-      <c r="AG4" s="45"/>
-    </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B5" s="53" t="s">
+      <c r="T4" s="64"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
+      <c r="W4" s="64"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="64"/>
+      <c r="AC4" s="64"/>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="65"/>
+    </row>
+    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B5" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="48"/>
+      <c r="G5" s="68"/>
       <c r="H5" s="2"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="44" t="s">
+      <c r="S5" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
-      <c r="X5" s="44"/>
-      <c r="Y5" s="44"/>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="44"/>
-      <c r="AB5" s="44"/>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="44"/>
-      <c r="AF5" s="44"/>
-      <c r="AG5" s="45"/>
-    </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="T5" s="64"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64"/>
+      <c r="W5" s="64"/>
+      <c r="X5" s="64"/>
+      <c r="Y5" s="64"/>
+      <c r="Z5" s="64"/>
+      <c r="AA5" s="64"/>
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="64"/>
+      <c r="AD5" s="64"/>
+      <c r="AE5" s="64"/>
+      <c r="AF5" s="64"/>
+      <c r="AG5" s="65"/>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B6" s="41"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="48"/>
+      <c r="G6" s="68"/>
       <c r="H6" s="2"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="49" t="s">
+      <c r="M6" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="44" t="s">
+      <c r="S6" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="T6" s="44"/>
-      <c r="U6" s="44"/>
-      <c r="V6" s="44"/>
-      <c r="W6" s="44"/>
-      <c r="X6" s="44"/>
-      <c r="Y6" s="44"/>
-      <c r="Z6" s="44"/>
-      <c r="AA6" s="44"/>
-      <c r="AB6" s="44"/>
-      <c r="AC6" s="44"/>
-      <c r="AD6" s="44"/>
-      <c r="AE6" s="44"/>
-      <c r="AF6" s="44"/>
-      <c r="AG6" s="45"/>
-    </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B7" s="54" t="s">
+      <c r="T6" s="64"/>
+      <c r="U6" s="64"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="64"/>
+      <c r="X6" s="64"/>
+      <c r="Y6" s="64"/>
+      <c r="Z6" s="64"/>
+      <c r="AA6" s="64"/>
+      <c r="AB6" s="64"/>
+      <c r="AC6" s="64"/>
+      <c r="AD6" s="64"/>
+      <c r="AE6" s="64"/>
+      <c r="AF6" s="64"/>
+      <c r="AG6" s="65"/>
+    </row>
+    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B7" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="48"/>
+      <c r="G7" s="68"/>
       <c r="H7" s="2"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="49" t="s">
+      <c r="M7" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="44" t="s">
+      <c r="S7" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="T7" s="44"/>
-      <c r="U7" s="44"/>
-      <c r="V7" s="44"/>
-      <c r="W7" s="44"/>
-      <c r="X7" s="44"/>
-      <c r="Y7" s="44"/>
-      <c r="Z7" s="44"/>
-      <c r="AA7" s="44"/>
-      <c r="AB7" s="44"/>
-      <c r="AC7" s="44"/>
-      <c r="AD7" s="44"/>
-      <c r="AE7" s="44"/>
-      <c r="AF7" s="44"/>
-      <c r="AG7" s="45"/>
-    </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="T7" s="64"/>
+      <c r="U7" s="64"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="64"/>
+      <c r="X7" s="64"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="64"/>
+      <c r="AA7" s="64"/>
+      <c r="AB7" s="64"/>
+      <c r="AC7" s="64"/>
+      <c r="AD7" s="64"/>
+      <c r="AE7" s="64"/>
+      <c r="AF7" s="64"/>
+      <c r="AG7" s="65"/>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B8" s="41"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="48"/>
+      <c r="G8" s="68"/>
       <c r="H8" s="2"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="49" t="s">
+      <c r="M8" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
+      <c r="N8" s="66"/>
+      <c r="O8" s="66"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="44" t="s">
+      <c r="S8" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="T8" s="44"/>
-      <c r="U8" s="44"/>
-      <c r="V8" s="44"/>
-      <c r="W8" s="44"/>
-      <c r="X8" s="44"/>
-      <c r="Y8" s="44"/>
-      <c r="Z8" s="44"/>
-      <c r="AA8" s="44"/>
-      <c r="AB8" s="44"/>
-      <c r="AC8" s="44"/>
-      <c r="AD8" s="44"/>
-      <c r="AE8" s="44"/>
-      <c r="AF8" s="44"/>
-      <c r="AG8" s="45"/>
-    </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="52"/>
+      <c r="T8" s="64"/>
+      <c r="U8" s="64"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="64"/>
+      <c r="X8" s="64"/>
+      <c r="Y8" s="64"/>
+      <c r="Z8" s="64"/>
+      <c r="AA8" s="64"/>
+      <c r="AB8" s="64"/>
+      <c r="AC8" s="64"/>
+      <c r="AD8" s="64"/>
+      <c r="AE8" s="64"/>
+      <c r="AF8" s="64"/>
+      <c r="AG8" s="65"/>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B9" s="74"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="76"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="48"/>
+      <c r="G9" s="68"/>
       <c r="H9" s="2"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="49" t="s">
+      <c r="M9" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="67"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="44" t="s">
+      <c r="S9" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="44"/>
-      <c r="Y9" s="44"/>
-      <c r="Z9" s="44"/>
-      <c r="AA9" s="44"/>
-      <c r="AB9" s="44"/>
-      <c r="AC9" s="44"/>
-      <c r="AD9" s="44"/>
-      <c r="AE9" s="44"/>
-      <c r="AF9" s="44"/>
-      <c r="AG9" s="45"/>
-    </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="T9" s="64"/>
+      <c r="U9" s="64"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="64"/>
+      <c r="X9" s="64"/>
+      <c r="Y9" s="64"/>
+      <c r="Z9" s="64"/>
+      <c r="AA9" s="64"/>
+      <c r="AB9" s="64"/>
+      <c r="AC9" s="64"/>
+      <c r="AD9" s="64"/>
+      <c r="AE9" s="64"/>
+      <c r="AF9" s="64"/>
+      <c r="AG9" s="65"/>
+    </row>
+    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B10" s="41"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1844,25 +2261,25 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="44" t="s">
+      <c r="S10" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="T10" s="44"/>
-      <c r="U10" s="44"/>
-      <c r="V10" s="44"/>
-      <c r="W10" s="44"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="44"/>
-      <c r="Z10" s="44"/>
-      <c r="AA10" s="44"/>
-      <c r="AB10" s="44"/>
-      <c r="AC10" s="44"/>
-      <c r="AD10" s="44"/>
-      <c r="AE10" s="44"/>
-      <c r="AF10" s="44"/>
-      <c r="AG10" s="45"/>
-    </row>
-    <row r="11" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T10" s="64"/>
+      <c r="U10" s="64"/>
+      <c r="V10" s="64"/>
+      <c r="W10" s="64"/>
+      <c r="X10" s="64"/>
+      <c r="Y10" s="64"/>
+      <c r="Z10" s="64"/>
+      <c r="AA10" s="64"/>
+      <c r="AB10" s="64"/>
+      <c r="AC10" s="64"/>
+      <c r="AD10" s="64"/>
+      <c r="AE10" s="64"/>
+      <c r="AF10" s="64"/>
+      <c r="AG10" s="65"/>
+    </row>
+    <row r="11" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="30"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1896,57 +2313,57 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="21"/>
     </row>
-    <row r="12" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="30"/>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="46" t="s">
+      <c r="K12" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="46" t="s">
+      <c r="O12" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
+      <c r="P12" s="72"/>
+      <c r="Q12" s="72"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="46" t="s">
+      <c r="S12" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
+      <c r="T12" s="72"/>
+      <c r="U12" s="72"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="46" t="s">
+      <c r="W12" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="X12" s="46"/>
-      <c r="Y12" s="46"/>
+      <c r="X12" s="72"/>
+      <c r="Y12" s="72"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="46" t="s">
+      <c r="AA12" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="AB12" s="46"/>
-      <c r="AC12" s="46"/>
+      <c r="AB12" s="72"/>
+      <c r="AC12" s="72"/>
       <c r="AD12" s="1"/>
-      <c r="AE12" s="46" t="s">
+      <c r="AE12" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="AF12" s="46"/>
-      <c r="AG12" s="47"/>
-    </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="AF12" s="72"/>
+      <c r="AG12" s="73"/>
+    </row>
+    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B13" s="30"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
@@ -1980,7 +2397,7 @@
       <c r="AF13" s="11"/>
       <c r="AG13" s="31"/>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B14" s="30"/>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
@@ -2014,7 +2431,7 @@
       <c r="AF14" s="11"/>
       <c r="AG14" s="32"/>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B15" s="30"/>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
@@ -2048,7 +2465,7 @@
       <c r="AF15" s="11"/>
       <c r="AG15" s="32"/>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B16" s="30"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
@@ -2082,7 +2499,7 @@
       <c r="AF16" s="11"/>
       <c r="AG16" s="32"/>
     </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B17" s="30"/>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
@@ -2116,7 +2533,7 @@
       <c r="AF17" s="11"/>
       <c r="AG17" s="32"/>
     </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B18" s="30"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
@@ -2150,7 +2567,7 @@
       <c r="AF18" s="11"/>
       <c r="AG18" s="32"/>
     </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B19" s="30"/>
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
@@ -2184,7 +2601,7 @@
       <c r="AF19" s="11"/>
       <c r="AG19" s="32"/>
     </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B20" s="30"/>
       <c r="C20" s="10"/>
       <c r="D20" s="11"/>
@@ -2218,7 +2635,7 @@
       <c r="AF20" s="11"/>
       <c r="AG20" s="32"/>
     </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B21" s="30"/>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
@@ -2252,7 +2669,7 @@
       <c r="AF21" s="11"/>
       <c r="AG21" s="32"/>
     </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B22" s="30"/>
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
@@ -2286,7 +2703,7 @@
       <c r="AF22" s="11"/>
       <c r="AG22" s="32"/>
     </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B23" s="30"/>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
@@ -2320,7 +2737,7 @@
       <c r="AF23" s="11"/>
       <c r="AG23" s="32"/>
     </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B24" s="30"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
@@ -2354,7 +2771,7 @@
       <c r="AF24" s="11"/>
       <c r="AG24" s="32"/>
     </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B25" s="30"/>
       <c r="C25" s="10"/>
       <c r="D25" s="11"/>
@@ -2388,7 +2805,7 @@
       <c r="AF25" s="11"/>
       <c r="AG25" s="32"/>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B26" s="30"/>
       <c r="C26" s="10"/>
       <c r="D26" s="11"/>
@@ -2422,7 +2839,7 @@
       <c r="AF26" s="11"/>
       <c r="AG26" s="32"/>
     </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B27" s="30"/>
       <c r="C27" s="10"/>
       <c r="D27" s="11"/>
@@ -2456,7 +2873,7 @@
       <c r="AF27" s="11"/>
       <c r="AG27" s="32"/>
     </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B28" s="30"/>
       <c r="C28" s="10"/>
       <c r="D28" s="11"/>
@@ -2490,7 +2907,7 @@
       <c r="AF28" s="11"/>
       <c r="AG28" s="32"/>
     </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B29" s="30"/>
       <c r="C29" s="10"/>
       <c r="D29" s="11"/>
@@ -2524,7 +2941,7 @@
       <c r="AF29" s="11"/>
       <c r="AG29" s="32"/>
     </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B30" s="30"/>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
@@ -2558,7 +2975,7 @@
       <c r="AF30" s="11"/>
       <c r="AG30" s="32"/>
     </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B31" s="30"/>
       <c r="C31" s="10"/>
       <c r="D31" s="11"/>
@@ -2592,7 +3009,7 @@
       <c r="AF31" s="11"/>
       <c r="AG31" s="32"/>
     </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B32" s="30"/>
       <c r="C32" s="10"/>
       <c r="D32" s="11"/>
@@ -2626,7 +3043,7 @@
       <c r="AF32" s="11"/>
       <c r="AG32" s="32"/>
     </row>
-    <row r="33" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B33" s="30"/>
       <c r="C33" s="10"/>
       <c r="D33" s="11"/>
@@ -2660,7 +3077,7 @@
       <c r="AF33" s="11"/>
       <c r="AG33" s="32"/>
     </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B34" s="30"/>
       <c r="C34" s="10"/>
       <c r="D34" s="11"/>
@@ -2694,7 +3111,7 @@
       <c r="AF34" s="11"/>
       <c r="AG34" s="32"/>
     </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B35" s="30"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
@@ -2728,7 +3145,7 @@
       <c r="AF35" s="11"/>
       <c r="AG35" s="32"/>
     </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B36" s="30"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
@@ -2762,7 +3179,7 @@
       <c r="AF36" s="11"/>
       <c r="AG36" s="32"/>
     </row>
-    <row r="37" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B37" s="30"/>
       <c r="C37" s="10"/>
       <c r="D37" s="11"/>
@@ -2796,7 +3213,7 @@
       <c r="AF37" s="11"/>
       <c r="AG37" s="32"/>
     </row>
-    <row r="38" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B38" s="30"/>
       <c r="C38" s="10"/>
       <c r="D38" s="11"/>
@@ -2830,7 +3247,7 @@
       <c r="AF38" s="11"/>
       <c r="AG38" s="32"/>
     </row>
-    <row r="39" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B39" s="30"/>
       <c r="C39" s="10"/>
       <c r="D39" s="11"/>
@@ -2864,7 +3281,7 @@
       <c r="AF39" s="11"/>
       <c r="AG39" s="32"/>
     </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B40" s="30"/>
       <c r="C40" s="10"/>
       <c r="D40" s="11"/>
@@ -2898,7 +3315,7 @@
       <c r="AF40" s="11"/>
       <c r="AG40" s="32"/>
     </row>
-    <row r="41" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B41" s="30"/>
       <c r="C41" s="10"/>
       <c r="D41" s="11"/>
@@ -2932,7 +3349,7 @@
       <c r="AF41" s="11"/>
       <c r="AG41" s="32"/>
     </row>
-    <row r="42" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B42" s="30"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
@@ -2966,7 +3383,7 @@
       <c r="AF42" s="11"/>
       <c r="AG42" s="32"/>
     </row>
-    <row r="43" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
@@ -3000,7 +3417,7 @@
       <c r="AF43" s="11"/>
       <c r="AG43" s="32"/>
     </row>
-    <row r="44" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B44" s="30"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
@@ -3034,7 +3451,7 @@
       <c r="AF44" s="11"/>
       <c r="AG44" s="32"/>
     </row>
-    <row r="45" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B45" s="30"/>
       <c r="C45" s="10"/>
       <c r="D45" s="11"/>
@@ -3068,7 +3485,7 @@
       <c r="AF45" s="11"/>
       <c r="AG45" s="32"/>
     </row>
-    <row r="46" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="33"/>
       <c r="C46" s="42"/>
       <c r="D46" s="35"/>
@@ -3102,15 +3519,25 @@
       <c r="AF46" s="35"/>
       <c r="AG46" s="37"/>
     </row>
-    <row r="47" spans="2:33" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B2:K3"/>
-    <mergeCell ref="S2:AG2"/>
-    <mergeCell ref="S3:AG3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="S4:AG4"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S7:AG7"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="W12:Y12"/>
+    <mergeCell ref="AA12:AC12"/>
+    <mergeCell ref="AE12:AG12"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="S9:AG9"/>
+    <mergeCell ref="S10:AG10"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="M8:O8"/>
     <mergeCell ref="P8:Q8"/>
@@ -3127,28 +3554,18 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="S7:AG7"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="W12:Y12"/>
-    <mergeCell ref="AA12:AC12"/>
-    <mergeCell ref="AE12:AG12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="S9:AG9"/>
-    <mergeCell ref="S10:AG10"/>
-    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="S2:AG2"/>
+    <mergeCell ref="S3:AG3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="S4:AG4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG47"/>
   <sheetViews>
@@ -3156,28 +3573,28 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.77734375" customWidth="1"/>
-    <col min="8" max="10" width="8.5546875" customWidth="1"/>
-    <col min="11" max="11" width="22.77734375" customWidth="1"/>
-    <col min="12" max="14" width="8.5546875" customWidth="1"/>
-    <col min="15" max="15" width="22.77734375" customWidth="1"/>
-    <col min="16" max="18" width="8.5546875" customWidth="1"/>
-    <col min="19" max="19" width="22.77734375" customWidth="1"/>
-    <col min="20" max="22" width="8.5546875" customWidth="1"/>
-    <col min="23" max="23" width="22.77734375" customWidth="1"/>
-    <col min="24" max="26" width="8.5546875" customWidth="1"/>
-    <col min="27" max="27" width="22.77734375" customWidth="1"/>
-    <col min="28" max="30" width="8.5546875" customWidth="1"/>
-    <col min="31" max="31" width="22.77734375" customWidth="1"/>
-    <col min="32" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="12" max="14" width="8.5703125" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" customWidth="1"/>
+    <col min="16" max="18" width="8.5703125" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" customWidth="1"/>
+    <col min="20" max="22" width="8.5703125" customWidth="1"/>
+    <col min="23" max="23" width="22.7109375" customWidth="1"/>
+    <col min="24" max="26" width="8.5703125" customWidth="1"/>
+    <col min="27" max="27" width="22.7109375" customWidth="1"/>
+    <col min="28" max="30" width="8.5703125" customWidth="1"/>
+    <col min="31" max="31" width="22.7109375" customWidth="1"/>
+    <col min="32" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -3211,20 +3628,20 @@
       <c r="AF1" s="22"/>
       <c r="AG1" s="22"/>
     </row>
-    <row r="2" spans="1:33" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
       <c r="N2" s="23"/>
@@ -3232,36 +3649,36 @@
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
-      <c r="S2" s="77" t="s">
+      <c r="S2" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="77"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="77"/>
-      <c r="W2" s="77"/>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="77"/>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="77"/>
-      <c r="AD2" s="77"/>
-      <c r="AE2" s="77"/>
-      <c r="AF2" s="77"/>
-      <c r="AG2" s="78"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
+      <c r="X2" s="90"/>
+      <c r="Y2" s="90"/>
+      <c r="Z2" s="90"/>
+      <c r="AA2" s="90"/>
+      <c r="AB2" s="90"/>
+      <c r="AC2" s="90"/>
+      <c r="AD2" s="90"/>
+      <c r="AE2" s="90"/>
+      <c r="AF2" s="90"/>
+      <c r="AG2" s="91"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
       <c r="L3" s="15"/>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
@@ -3269,25 +3686,25 @@
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
       <c r="R3" s="15"/>
-      <c r="S3" s="66" t="s">
+      <c r="S3" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="66"/>
-      <c r="U3" s="66"/>
-      <c r="V3" s="66"/>
-      <c r="W3" s="66"/>
-      <c r="X3" s="66"/>
-      <c r="Y3" s="66"/>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="66"/>
-      <c r="AB3" s="66"/>
-      <c r="AC3" s="66"/>
-      <c r="AD3" s="66"/>
-      <c r="AE3" s="66"/>
-      <c r="AF3" s="66"/>
-      <c r="AG3" s="67"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
+      <c r="AE3" s="83"/>
+      <c r="AF3" s="83"/>
+      <c r="AG3" s="84"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="24"/>
       <c r="C4" s="15"/>
@@ -3300,242 +3717,242 @@
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="68" t="s">
+      <c r="M4" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
       <c r="R4" s="15"/>
-      <c r="S4" s="66" t="s">
+      <c r="S4" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="66"/>
-      <c r="W4" s="66"/>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="66"/>
-      <c r="AA4" s="66"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="66"/>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="66"/>
-      <c r="AG4" s="67"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T4" s="83"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="83"/>
+      <c r="W4" s="83"/>
+      <c r="X4" s="83"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="83"/>
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="83"/>
+      <c r="AC4" s="83"/>
+      <c r="AD4" s="83"/>
+      <c r="AE4" s="83"/>
+      <c r="AF4" s="83"/>
+      <c r="AG4" s="84"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="69"/>
+      <c r="G5" s="95"/>
       <c r="H5" s="38"/>
       <c r="I5" s="15"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="68" t="s">
+      <c r="M5" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
       <c r="R5" s="15"/>
-      <c r="S5" s="66" t="s">
+      <c r="S5" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="66"/>
-      <c r="Z5" s="66"/>
-      <c r="AA5" s="66"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
-      <c r="AD5" s="66"/>
-      <c r="AE5" s="66"/>
-      <c r="AF5" s="66"/>
-      <c r="AG5" s="67"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="83"/>
+      <c r="AB5" s="83"/>
+      <c r="AC5" s="83"/>
+      <c r="AD5" s="83"/>
+      <c r="AE5" s="83"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="84"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="24"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
-      <c r="F6" s="62" t="s">
+      <c r="F6" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="62"/>
+      <c r="G6" s="77"/>
       <c r="H6" s="38"/>
       <c r="I6" s="15"/>
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="68" t="s">
+      <c r="M6" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
       <c r="R6" s="15"/>
-      <c r="S6" s="66" t="s">
+      <c r="S6" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="T6" s="66"/>
-      <c r="U6" s="66"/>
-      <c r="V6" s="66"/>
-      <c r="W6" s="66"/>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="66"/>
-      <c r="Z6" s="66"/>
-      <c r="AA6" s="66"/>
-      <c r="AB6" s="66"/>
-      <c r="AC6" s="66"/>
-      <c r="AD6" s="66"/>
-      <c r="AE6" s="66"/>
-      <c r="AF6" s="66"/>
-      <c r="AG6" s="67"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T6" s="83"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="83"/>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="83"/>
+      <c r="Z6" s="83"/>
+      <c r="AA6" s="83"/>
+      <c r="AB6" s="83"/>
+      <c r="AC6" s="83"/>
+      <c r="AD6" s="83"/>
+      <c r="AE6" s="83"/>
+      <c r="AF6" s="83"/>
+      <c r="AG6" s="84"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="62" t="s">
+      <c r="F7" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="62"/>
+      <c r="G7" s="77"/>
       <c r="H7" s="38"/>
       <c r="I7" s="15"/>
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="68" t="s">
+      <c r="M7" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="72"/>
+      <c r="N7" s="85"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
       <c r="R7" s="15"/>
-      <c r="S7" s="66" t="s">
+      <c r="S7" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="T7" s="66"/>
-      <c r="U7" s="66"/>
-      <c r="V7" s="66"/>
-      <c r="W7" s="66"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="66"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
-      <c r="AB7" s="66"/>
-      <c r="AC7" s="66"/>
-      <c r="AD7" s="66"/>
-      <c r="AE7" s="66"/>
-      <c r="AF7" s="66"/>
-      <c r="AG7" s="67"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="83"/>
+      <c r="AA7" s="83"/>
+      <c r="AB7" s="83"/>
+      <c r="AC7" s="83"/>
+      <c r="AD7" s="83"/>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="84"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="24"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="62"/>
+      <c r="G8" s="77"/>
       <c r="H8" s="38"/>
       <c r="I8" s="15"/>
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="68" t="s">
+      <c r="M8" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
+      <c r="N8" s="85"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="82"/>
       <c r="R8" s="15"/>
-      <c r="S8" s="66" t="s">
+      <c r="S8" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="T8" s="66"/>
-      <c r="U8" s="66"/>
-      <c r="V8" s="66"/>
-      <c r="W8" s="66"/>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="66"/>
-      <c r="AC8" s="66"/>
-      <c r="AD8" s="66"/>
-      <c r="AE8" s="66"/>
-      <c r="AF8" s="66"/>
-      <c r="AG8" s="67"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="T8" s="83"/>
+      <c r="U8" s="83"/>
+      <c r="V8" s="83"/>
+      <c r="W8" s="83"/>
+      <c r="X8" s="83"/>
+      <c r="Y8" s="83"/>
+      <c r="Z8" s="83"/>
+      <c r="AA8" s="83"/>
+      <c r="AB8" s="83"/>
+      <c r="AC8" s="83"/>
+      <c r="AD8" s="83"/>
+      <c r="AE8" s="83"/>
+      <c r="AF8" s="83"/>
+      <c r="AG8" s="84"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="65"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="62"/>
+      <c r="G9" s="77"/>
       <c r="H9" s="38"/>
       <c r="I9" s="15"/>
       <c r="J9" s="39"/>
       <c r="K9" s="39"/>
       <c r="L9" s="15"/>
-      <c r="M9" s="68" t="s">
+      <c r="M9" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="68"/>
-      <c r="O9" s="68"/>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="72"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="82"/>
+      <c r="Q9" s="82"/>
       <c r="R9" s="15"/>
-      <c r="S9" s="66" t="s">
+      <c r="S9" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="T9" s="66"/>
-      <c r="U9" s="66"/>
-      <c r="V9" s="66"/>
-      <c r="W9" s="66"/>
-      <c r="X9" s="66"/>
-      <c r="Y9" s="66"/>
-      <c r="Z9" s="66"/>
-      <c r="AA9" s="66"/>
-      <c r="AB9" s="66"/>
-      <c r="AC9" s="66"/>
-      <c r="AD9" s="66"/>
-      <c r="AE9" s="66"/>
-      <c r="AF9" s="66"/>
-      <c r="AG9" s="67"/>
-    </row>
-    <row r="10" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T9" s="83"/>
+      <c r="U9" s="83"/>
+      <c r="V9" s="83"/>
+      <c r="W9" s="83"/>
+      <c r="X9" s="83"/>
+      <c r="Y9" s="83"/>
+      <c r="Z9" s="83"/>
+      <c r="AA9" s="83"/>
+      <c r="AB9" s="83"/>
+      <c r="AC9" s="83"/>
+      <c r="AD9" s="83"/>
+      <c r="AE9" s="83"/>
+      <c r="AF9" s="83"/>
+      <c r="AG9" s="84"/>
+    </row>
+    <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="25"/>
       <c r="C10" s="26"/>
@@ -3554,25 +3971,25 @@
       <c r="P10" s="26"/>
       <c r="Q10" s="26"/>
       <c r="R10" s="26"/>
-      <c r="S10" s="81" t="s">
+      <c r="S10" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="T10" s="81"/>
-      <c r="U10" s="81"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="81"/>
-      <c r="Z10" s="81"/>
-      <c r="AA10" s="81"/>
-      <c r="AB10" s="81"/>
-      <c r="AC10" s="81"/>
-      <c r="AD10" s="81"/>
-      <c r="AE10" s="81"/>
-      <c r="AF10" s="81"/>
-      <c r="AG10" s="82"/>
-    </row>
-    <row r="11" spans="1:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T10" s="78"/>
+      <c r="U10" s="78"/>
+      <c r="V10" s="78"/>
+      <c r="W10" s="78"/>
+      <c r="X10" s="78"/>
+      <c r="Y10" s="78"/>
+      <c r="Z10" s="78"/>
+      <c r="AA10" s="78"/>
+      <c r="AB10" s="78"/>
+      <c r="AC10" s="78"/>
+      <c r="AD10" s="78"/>
+      <c r="AE10" s="78"/>
+      <c r="AF10" s="78"/>
+      <c r="AG10" s="79"/>
+    </row>
+    <row r="11" spans="1:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="27"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
@@ -3606,57 +4023,57 @@
       <c r="AF11" s="28"/>
       <c r="AG11" s="29"/>
     </row>
-    <row r="12" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="30"/>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="83" t="s">
+      <c r="G12" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="83" t="s">
+      <c r="K12" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="83"/>
-      <c r="M12" s="83"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="83" t="s">
+      <c r="O12" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="83"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="80"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="83" t="s">
+      <c r="S12" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="T12" s="83"/>
-      <c r="U12" s="83"/>
+      <c r="T12" s="80"/>
+      <c r="U12" s="80"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="83" t="s">
+      <c r="W12" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="X12" s="83"/>
-      <c r="Y12" s="83"/>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="80"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="83" t="s">
+      <c r="AA12" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="AB12" s="83"/>
-      <c r="AC12" s="83"/>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="80"/>
       <c r="AD12" s="1"/>
-      <c r="AE12" s="83" t="s">
+      <c r="AE12" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="AF12" s="83"/>
-      <c r="AG12" s="84"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AF12" s="80"/>
+      <c r="AG12" s="81"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" s="30"/>
       <c r="C13" s="19"/>
       <c r="D13" s="8"/>
@@ -3690,7 +4107,7 @@
       <c r="AF13" s="11"/>
       <c r="AG13" s="31"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="30"/>
       <c r="C14" s="20"/>
       <c r="D14" s="11"/>
@@ -3724,7 +4141,7 @@
       <c r="AF14" s="11"/>
       <c r="AG14" s="32"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" s="30"/>
       <c r="C15" s="20"/>
       <c r="D15" s="11"/>
@@ -3758,7 +4175,7 @@
       <c r="AF15" s="11"/>
       <c r="AG15" s="32"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" s="30"/>
       <c r="C16" s="20"/>
       <c r="D16" s="11"/>
@@ -3792,7 +4209,7 @@
       <c r="AF16" s="11"/>
       <c r="AG16" s="32"/>
     </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B17" s="30"/>
       <c r="C17" s="20"/>
       <c r="D17" s="11"/>
@@ -3826,7 +4243,7 @@
       <c r="AF17" s="11"/>
       <c r="AG17" s="32"/>
     </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B18" s="30"/>
       <c r="C18" s="20"/>
       <c r="D18" s="11"/>
@@ -3860,7 +4277,7 @@
       <c r="AF18" s="11"/>
       <c r="AG18" s="32"/>
     </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B19" s="30"/>
       <c r="C19" s="20"/>
       <c r="D19" s="11"/>
@@ -3894,7 +4311,7 @@
       <c r="AF19" s="11"/>
       <c r="AG19" s="32"/>
     </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B20" s="30"/>
       <c r="C20" s="20"/>
       <c r="D20" s="11"/>
@@ -3928,7 +4345,7 @@
       <c r="AF20" s="11"/>
       <c r="AG20" s="32"/>
     </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B21" s="30"/>
       <c r="C21" s="20"/>
       <c r="D21" s="11"/>
@@ -3962,7 +4379,7 @@
       <c r="AF21" s="11"/>
       <c r="AG21" s="32"/>
     </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B22" s="30"/>
       <c r="C22" s="20"/>
       <c r="D22" s="11"/>
@@ -3996,7 +4413,7 @@
       <c r="AF22" s="11"/>
       <c r="AG22" s="32"/>
     </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B23" s="30"/>
       <c r="C23" s="20"/>
       <c r="D23" s="11"/>
@@ -4030,7 +4447,7 @@
       <c r="AF23" s="11"/>
       <c r="AG23" s="32"/>
     </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B24" s="30"/>
       <c r="C24" s="20"/>
       <c r="D24" s="11"/>
@@ -4064,7 +4481,7 @@
       <c r="AF24" s="11"/>
       <c r="AG24" s="32"/>
     </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B25" s="30"/>
       <c r="C25" s="20"/>
       <c r="D25" s="11"/>
@@ -4098,7 +4515,7 @@
       <c r="AF25" s="11"/>
       <c r="AG25" s="32"/>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B26" s="30"/>
       <c r="C26" s="20"/>
       <c r="D26" s="11"/>
@@ -4132,7 +4549,7 @@
       <c r="AF26" s="11"/>
       <c r="AG26" s="32"/>
     </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B27" s="30"/>
       <c r="C27" s="20"/>
       <c r="D27" s="11"/>
@@ -4166,7 +4583,7 @@
       <c r="AF27" s="11"/>
       <c r="AG27" s="32"/>
     </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B28" s="30"/>
       <c r="C28" s="20"/>
       <c r="D28" s="11"/>
@@ -4200,7 +4617,7 @@
       <c r="AF28" s="11"/>
       <c r="AG28" s="32"/>
     </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B29" s="30"/>
       <c r="C29" s="20"/>
       <c r="D29" s="11"/>
@@ -4234,7 +4651,7 @@
       <c r="AF29" s="11"/>
       <c r="AG29" s="32"/>
     </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B30" s="30"/>
       <c r="C30" s="20"/>
       <c r="D30" s="11"/>
@@ -4268,7 +4685,7 @@
       <c r="AF30" s="11"/>
       <c r="AG30" s="32"/>
     </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B31" s="30"/>
       <c r="C31" s="20"/>
       <c r="D31" s="11"/>
@@ -4302,7 +4719,7 @@
       <c r="AF31" s="11"/>
       <c r="AG31" s="32"/>
     </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B32" s="30"/>
       <c r="C32" s="20"/>
       <c r="D32" s="11"/>
@@ -4336,7 +4753,7 @@
       <c r="AF32" s="11"/>
       <c r="AG32" s="32"/>
     </row>
-    <row r="33" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B33" s="30"/>
       <c r="C33" s="20"/>
       <c r="D33" s="11"/>
@@ -4370,7 +4787,7 @@
       <c r="AF33" s="11"/>
       <c r="AG33" s="32"/>
     </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B34" s="30"/>
       <c r="C34" s="20"/>
       <c r="D34" s="11"/>
@@ -4404,7 +4821,7 @@
       <c r="AF34" s="11"/>
       <c r="AG34" s="32"/>
     </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B35" s="30"/>
       <c r="C35" s="20"/>
       <c r="D35" s="11"/>
@@ -4438,7 +4855,7 @@
       <c r="AF35" s="11"/>
       <c r="AG35" s="32"/>
     </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B36" s="30"/>
       <c r="C36" s="20"/>
       <c r="D36" s="11"/>
@@ -4472,7 +4889,7 @@
       <c r="AF36" s="11"/>
       <c r="AG36" s="32"/>
     </row>
-    <row r="37" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B37" s="30"/>
       <c r="C37" s="20"/>
       <c r="D37" s="11"/>
@@ -4506,7 +4923,7 @@
       <c r="AF37" s="11"/>
       <c r="AG37" s="32"/>
     </row>
-    <row r="38" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B38" s="30"/>
       <c r="C38" s="20"/>
       <c r="D38" s="11"/>
@@ -4540,7 +4957,7 @@
       <c r="AF38" s="11"/>
       <c r="AG38" s="32"/>
     </row>
-    <row r="39" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B39" s="30"/>
       <c r="C39" s="20"/>
       <c r="D39" s="11"/>
@@ -4574,7 +4991,7 @@
       <c r="AF39" s="11"/>
       <c r="AG39" s="32"/>
     </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B40" s="30"/>
       <c r="C40" s="20"/>
       <c r="D40" s="11"/>
@@ -4608,7 +5025,7 @@
       <c r="AF40" s="11"/>
       <c r="AG40" s="32"/>
     </row>
-    <row r="41" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B41" s="30"/>
       <c r="C41" s="20"/>
       <c r="D41" s="11"/>
@@ -4642,7 +5059,7 @@
       <c r="AF41" s="11"/>
       <c r="AG41" s="32"/>
     </row>
-    <row r="42" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B42" s="30"/>
       <c r="C42" s="20"/>
       <c r="D42" s="11"/>
@@ -4676,7 +5093,7 @@
       <c r="AF42" s="11"/>
       <c r="AG42" s="32"/>
     </row>
-    <row r="43" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
       <c r="C43" s="20"/>
       <c r="D43" s="11"/>
@@ -4710,7 +5127,7 @@
       <c r="AF43" s="11"/>
       <c r="AG43" s="32"/>
     </row>
-    <row r="44" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B44" s="30"/>
       <c r="C44" s="20"/>
       <c r="D44" s="11"/>
@@ -4744,7 +5161,7 @@
       <c r="AF44" s="11"/>
       <c r="AG44" s="32"/>
     </row>
-    <row r="45" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B45" s="30"/>
       <c r="C45" s="20"/>
       <c r="D45" s="11"/>
@@ -4778,7 +5195,7 @@
       <c r="AF45" s="11"/>
       <c r="AG45" s="32"/>
     </row>
-    <row r="46" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="33"/>
       <c r="C46" s="34"/>
       <c r="D46" s="35"/>
@@ -4812,33 +5229,9 @@
       <c r="AF46" s="35"/>
       <c r="AG46" s="37"/>
     </row>
-    <row r="47" spans="2:33" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="S10:AG10"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="W12:Y12"/>
-    <mergeCell ref="AA12:AC12"/>
-    <mergeCell ref="AE12:AG12"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="S8:AG8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="S9:AG9"/>
-    <mergeCell ref="B2:K3"/>
-    <mergeCell ref="S2:AG2"/>
-    <mergeCell ref="S3:AG3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="S4:AG4"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="S5:AG5"/>
     <mergeCell ref="M6:O6"/>
@@ -4853,68 +5246,92 @@
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="S7:AG7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="S2:AG2"/>
+    <mergeCell ref="S3:AG3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="S4:AG4"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="S10:AG10"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="W12:Y12"/>
+    <mergeCell ref="AA12:AC12"/>
+    <mergeCell ref="AE12:AG12"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="S8:AG8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="S9:AG9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031F73E0-D27C-4EE3-9EBC-BB02AFC3DE51}">
   <dimension ref="B2:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="101" t="s">
+    <row r="2" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="102"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="102"/>
-      <c r="S2" s="103"/>
-    </row>
-    <row r="3" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="104"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="106"/>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="114"/>
+    </row>
+    <row r="3" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="115"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="116"/>
+      <c r="P3" s="116"/>
+      <c r="Q3" s="116"/>
+      <c r="R3" s="116"/>
+      <c r="S3" s="117"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="16"/>
@@ -4931,132 +5348,132 @@
       <c r="O4" s="15"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
-      <c r="R4" s="107"/>
-      <c r="S4" s="107"/>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B5" s="98" t="s">
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="100"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="123"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="95" t="s">
+      <c r="G5" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="96"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="65"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="132"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="94" t="s">
+      <c r="M5" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="94"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="124"/>
+      <c r="Q5" s="125"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="95" t="s">
+      <c r="G6" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="96"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="65"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="125"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="94" t="s">
+      <c r="M6" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="94"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="85"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="98"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="100"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="126"/>
+      <c r="P6" s="131"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="121"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="123"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="95" t="s">
+      <c r="G7" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="96"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="65"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="120"/>
+      <c r="J7" s="133"/>
+      <c r="K7" s="94"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="94" t="s">
+      <c r="M7" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="65"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="N7" s="126"/>
+      <c r="O7" s="126"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="132"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="43"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="95" t="s">
+      <c r="G8" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="96"/>
-      <c r="I8" s="97"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="65"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="131"/>
+      <c r="K8" s="132"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="94" t="s">
+      <c r="M8" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="94"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="85"/>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="107"/>
-      <c r="S8" s="107"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="98"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="100"/>
+      <c r="N8" s="126"/>
+      <c r="O8" s="126"/>
+      <c r="P8" s="124"/>
+      <c r="Q8" s="125"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="121"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="123"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="95" t="s">
+      <c r="G9" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="96"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="65"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="131"/>
+      <c r="K9" s="132"/>
       <c r="L9" s="15"/>
-      <c r="M9" s="94" t="s">
+      <c r="M9" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="107"/>
-      <c r="S9" s="107"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="N9" s="126"/>
+      <c r="O9" s="126"/>
+      <c r="P9" s="133"/>
+      <c r="Q9" s="94"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -5073,58 +5490,76 @@
       <c r="O10" s="15"/>
       <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
-      <c r="R10" s="107"/>
-      <c r="S10" s="107"/>
-    </row>
-    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:19" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C12" s="108" t="s">
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+    </row>
+    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:19" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="108" t="s">
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="109"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="108" t="s">
+      <c r="H12" s="107"/>
+      <c r="I12" s="108"/>
+      <c r="J12" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="109"/>
-      <c r="L12" s="110"/>
-      <c r="M12" s="89" t="s">
+      <c r="K12" s="107"/>
+      <c r="L12" s="108"/>
+      <c r="M12" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="90"/>
-      <c r="O12" s="91"/>
-      <c r="P12" s="89" t="s">
+      <c r="N12" s="104"/>
+      <c r="O12" s="105"/>
+      <c r="P12" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="91"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="C13" s="86"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="92"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="93"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="87"/>
-      <c r="R13" s="93"/>
+      <c r="Q12" s="104"/>
+      <c r="R12" s="105"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C13" s="127"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="110"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="128"/>
+      <c r="N13" s="129"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="100"/>
+      <c r="Q13" s="101"/>
+      <c r="R13" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
     <mergeCell ref="P13:R13"/>
     <mergeCell ref="P12:R12"/>
     <mergeCell ref="G12:I12"/>
@@ -5141,24 +5576,6 @@
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
We mergin - updated Templates.xlsx to fix view position and zoom Speech - ChestRecognizer does not work now - removed unused code from EnemyHandling - SessionSheet now inserts grammar name into the spreadsheet to ease merging - modified Advance() to indicate whether it moved to new column Sync - added testing session data - MergeHelper now correctly merges session into main yay
</commit_message>
<xml_diff>
--- a/Templates/Templates.xlsx
+++ b/Templates/Templates.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Metin2DropAnalyzer\Metin2SpeechToData\bin\Debug\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B687507-ABB4-4387-BCBB-8EE266342188}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5926E3D2-04D1-4F9B-A4BC-F7563EEDECC8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="7" r:id="rId1"/>
     <sheet name="Area" sheetId="5" r:id="rId2"/>
-    <sheet name="Enemy" sheetId="2" r:id="rId3"/>
+    <sheet name="Enemy" sheetId="8" r:id="rId3"/>
     <sheet name="Session" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017" iterateDelta="1E-4"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <r>
       <rPr>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Metin2 siNDiCATE Drop Analyzer/Logger</t>
+  </si>
+  <si>
+    <t>_SESSION_AREA</t>
   </si>
 </sst>
 </file>
@@ -1067,6 +1070,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1092,6 +1098,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1142,23 +1157,47 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1173,30 +1212,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1297,18 +1312,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1700,78 +1703,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D37D157-3B5C-4918-9447-DD7F6F6CF083}">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="51"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="53"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="54"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
-      <c r="U4" s="56"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="57"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
@@ -1779,45 +1782,45 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
-      <c r="D6" s="134" t="s">
+      <c r="D6" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="136"/>
-      <c r="J6" s="134" t="s">
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="60"/>
+      <c r="J6" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="136"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="60"/>
       <c r="N6" s="44"/>
       <c r="O6" s="44"/>
-      <c r="P6" s="134" t="s">
+      <c r="P6" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="136"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="60"/>
       <c r="U6" s="21"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="C7" s="44"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="137"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
       <c r="H7" s="44"/>
       <c r="I7" s="44"/>
-      <c r="J7" s="137"/>
-      <c r="K7" s="137"/>
-      <c r="L7" s="137"/>
-      <c r="M7" s="137"/>
-      <c r="P7" s="137"/>
-      <c r="Q7" s="137"/>
-      <c r="R7" s="137"/>
-      <c r="S7" s="137"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
       <c r="U7" s="21"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1910,9 +1913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E4C1B2-82A3-4D72-8863-46DE92AE18FA}">
   <dimension ref="B1:AG47"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:AG2"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1928,18 +1929,18 @@
   <sheetData>
     <row r="1" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
       <c r="L2" s="40"/>
       <c r="M2" s="40"/>
       <c r="N2" s="40"/>
@@ -1947,35 +1948,35 @@
       <c r="P2" s="40"/>
       <c r="Q2" s="40"/>
       <c r="R2" s="40"/>
-      <c r="S2" s="61" t="s">
+      <c r="S2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="61"/>
-      <c r="W2" s="61"/>
-      <c r="X2" s="61"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
-      <c r="AC2" s="61"/>
-      <c r="AD2" s="61"/>
-      <c r="AE2" s="61"/>
-      <c r="AF2" s="61"/>
-      <c r="AG2" s="62"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="66"/>
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="L3" s="2"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -1983,23 +1984,23 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="63" t="s">
+      <c r="S3" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="65"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
+      <c r="X3" s="68"/>
+      <c r="Y3" s="68"/>
+      <c r="Z3" s="68"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="69"/>
     </row>
     <row r="4" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B4" s="41"/>
@@ -2013,235 +2014,235 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="66" t="s">
+      <c r="M4" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="63" t="s">
+      <c r="S4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="64"/>
-      <c r="AA4" s="64"/>
-      <c r="AB4" s="64"/>
-      <c r="AC4" s="64"/>
-      <c r="AD4" s="64"/>
-      <c r="AE4" s="64"/>
-      <c r="AF4" s="64"/>
-      <c r="AG4" s="65"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
+      <c r="Y4" s="68"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="68"/>
+      <c r="AC4" s="68"/>
+      <c r="AD4" s="68"/>
+      <c r="AE4" s="68"/>
+      <c r="AF4" s="68"/>
+      <c r="AG4" s="69"/>
     </row>
     <row r="5" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="68"/>
+      <c r="G5" s="72"/>
       <c r="H5" s="2"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="66" t="s">
+      <c r="M5" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="71"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="63" t="s">
+      <c r="S5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="64"/>
-      <c r="Z5" s="64"/>
-      <c r="AA5" s="64"/>
-      <c r="AB5" s="64"/>
-      <c r="AC5" s="64"/>
-      <c r="AD5" s="64"/>
-      <c r="AE5" s="64"/>
-      <c r="AF5" s="64"/>
-      <c r="AG5" s="65"/>
+      <c r="T5" s="68"/>
+      <c r="U5" s="68"/>
+      <c r="V5" s="68"/>
+      <c r="W5" s="68"/>
+      <c r="X5" s="68"/>
+      <c r="Y5" s="68"/>
+      <c r="Z5" s="68"/>
+      <c r="AA5" s="68"/>
+      <c r="AB5" s="68"/>
+      <c r="AC5" s="68"/>
+      <c r="AD5" s="68"/>
+      <c r="AE5" s="68"/>
+      <c r="AF5" s="68"/>
+      <c r="AG5" s="69"/>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B6" s="41"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="68"/>
+      <c r="G6" s="72"/>
       <c r="H6" s="2"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="66" t="s">
+      <c r="M6" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="63" t="s">
+      <c r="S6" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="T6" s="64"/>
-      <c r="U6" s="64"/>
-      <c r="V6" s="64"/>
-      <c r="W6" s="64"/>
-      <c r="X6" s="64"/>
-      <c r="Y6" s="64"/>
-      <c r="Z6" s="64"/>
-      <c r="AA6" s="64"/>
-      <c r="AB6" s="64"/>
-      <c r="AC6" s="64"/>
-      <c r="AD6" s="64"/>
-      <c r="AE6" s="64"/>
-      <c r="AF6" s="64"/>
-      <c r="AG6" s="65"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="68"/>
+      <c r="W6" s="68"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="68"/>
+      <c r="Z6" s="68"/>
+      <c r="AA6" s="68"/>
+      <c r="AB6" s="68"/>
+      <c r="AC6" s="68"/>
+      <c r="AD6" s="68"/>
+      <c r="AE6" s="68"/>
+      <c r="AF6" s="68"/>
+      <c r="AG6" s="69"/>
     </row>
     <row r="7" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="68"/>
+      <c r="G7" s="72"/>
       <c r="H7" s="2"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="66" t="s">
+      <c r="M7" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="71"/>
+      <c r="Q7" s="71"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="63" t="s">
+      <c r="S7" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="64"/>
-      <c r="AC7" s="64"/>
-      <c r="AD7" s="64"/>
-      <c r="AE7" s="64"/>
-      <c r="AF7" s="64"/>
-      <c r="AG7" s="65"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="68"/>
+      <c r="V7" s="68"/>
+      <c r="W7" s="68"/>
+      <c r="X7" s="68"/>
+      <c r="Y7" s="68"/>
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="68"/>
+      <c r="AC7" s="68"/>
+      <c r="AD7" s="68"/>
+      <c r="AE7" s="68"/>
+      <c r="AF7" s="68"/>
+      <c r="AG7" s="69"/>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B8" s="41"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="68"/>
+      <c r="G8" s="72"/>
       <c r="H8" s="2"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="66" t="s">
+      <c r="M8" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="67"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="70"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="63" t="s">
+      <c r="S8" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="T8" s="64"/>
-      <c r="U8" s="64"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="64"/>
-      <c r="X8" s="64"/>
-      <c r="Y8" s="64"/>
-      <c r="Z8" s="64"/>
-      <c r="AA8" s="64"/>
-      <c r="AB8" s="64"/>
-      <c r="AC8" s="64"/>
-      <c r="AD8" s="64"/>
-      <c r="AE8" s="64"/>
-      <c r="AF8" s="64"/>
-      <c r="AG8" s="65"/>
+      <c r="T8" s="68"/>
+      <c r="U8" s="68"/>
+      <c r="V8" s="68"/>
+      <c r="W8" s="68"/>
+      <c r="X8" s="68"/>
+      <c r="Y8" s="68"/>
+      <c r="Z8" s="68"/>
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="68"/>
+      <c r="AC8" s="68"/>
+      <c r="AD8" s="68"/>
+      <c r="AE8" s="68"/>
+      <c r="AF8" s="68"/>
+      <c r="AG8" s="69"/>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B9" s="74"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="76"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="80"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="68" t="s">
+      <c r="F9" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="68"/>
+      <c r="G9" s="72"/>
       <c r="H9" s="2"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="66" t="s">
+      <c r="M9" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="66"/>
-      <c r="O9" s="66"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="67"/>
+      <c r="N9" s="70"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="71"/>
+      <c r="Q9" s="71"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="63" t="s">
+      <c r="S9" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="T9" s="64"/>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="64"/>
-      <c r="AA9" s="64"/>
-      <c r="AB9" s="64"/>
-      <c r="AC9" s="64"/>
-      <c r="AD9" s="64"/>
-      <c r="AE9" s="64"/>
-      <c r="AF9" s="64"/>
-      <c r="AG9" s="65"/>
+      <c r="T9" s="68"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="68"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="68"/>
+      <c r="Y9" s="68"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="68"/>
+      <c r="AC9" s="68"/>
+      <c r="AD9" s="68"/>
+      <c r="AE9" s="68"/>
+      <c r="AF9" s="68"/>
+      <c r="AG9" s="69"/>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B10" s="41"/>
@@ -2261,23 +2262,23 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="63" t="s">
+      <c r="S10" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="T10" s="64"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="64"/>
-      <c r="X10" s="64"/>
-      <c r="Y10" s="64"/>
-      <c r="Z10" s="64"/>
-      <c r="AA10" s="64"/>
-      <c r="AB10" s="64"/>
-      <c r="AC10" s="64"/>
-      <c r="AD10" s="64"/>
-      <c r="AE10" s="64"/>
-      <c r="AF10" s="64"/>
-      <c r="AG10" s="65"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="68"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="68"/>
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="68"/>
+      <c r="AC10" s="68"/>
+      <c r="AD10" s="68"/>
+      <c r="AE10" s="68"/>
+      <c r="AF10" s="68"/>
+      <c r="AG10" s="69"/>
     </row>
     <row r="11" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="30"/>
@@ -2315,53 +2316,53 @@
     </row>
     <row r="12" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="30"/>
-      <c r="C12" s="72" t="s">
+      <c r="C12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="72" t="s">
+      <c r="G12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="72" t="s">
+      <c r="K12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="72" t="s">
+      <c r="O12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="72"/>
-      <c r="Q12" s="72"/>
+      <c r="P12" s="76"/>
+      <c r="Q12" s="76"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="72" t="s">
+      <c r="S12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="T12" s="72"/>
-      <c r="U12" s="72"/>
+      <c r="T12" s="76"/>
+      <c r="U12" s="76"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="72" t="s">
+      <c r="W12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="X12" s="72"/>
-      <c r="Y12" s="72"/>
+      <c r="X12" s="76"/>
+      <c r="Y12" s="76"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="72" t="s">
+      <c r="AA12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="AB12" s="72"/>
-      <c r="AC12" s="72"/>
+      <c r="AB12" s="76"/>
+      <c r="AC12" s="76"/>
       <c r="AD12" s="1"/>
-      <c r="AE12" s="72" t="s">
+      <c r="AE12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="AF12" s="72"/>
-      <c r="AG12" s="73"/>
+      <c r="AF12" s="76"/>
+      <c r="AG12" s="77"/>
     </row>
     <row r="13" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B13" s="30"/>
@@ -3566,35 +3567,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AG47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B79D6F-32D7-4B80-9D11-9180F3EB2F60}">
+  <dimension ref="A1:AH47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="10" width="8.5703125" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
-    <col min="12" max="14" width="8.5703125" customWidth="1"/>
-    <col min="15" max="15" width="22.7109375" customWidth="1"/>
-    <col min="16" max="18" width="8.5703125" customWidth="1"/>
-    <col min="19" max="19" width="22.7109375" customWidth="1"/>
-    <col min="20" max="22" width="8.5703125" customWidth="1"/>
-    <col min="23" max="23" width="22.7109375" customWidth="1"/>
-    <col min="24" max="26" width="8.5703125" customWidth="1"/>
-    <col min="27" max="27" width="22.7109375" customWidth="1"/>
-    <col min="28" max="30" width="8.5703125" customWidth="1"/>
-    <col min="31" max="31" width="22.7109375" customWidth="1"/>
-    <col min="32" max="1025" width="8.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -3627,21 +3608,22 @@
       <c r="AE1" s="22"/>
       <c r="AF1" s="22"/>
       <c r="AG1" s="22"/>
-    </row>
-    <row r="2" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AH1" s="14"/>
+    </row>
+    <row r="2" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
       <c r="N2" s="23"/>
@@ -3649,36 +3631,37 @@
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
       <c r="R2" s="23"/>
-      <c r="S2" s="90" t="s">
+      <c r="S2" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="90"/>
-      <c r="Y2" s="90"/>
-      <c r="Z2" s="90"/>
-      <c r="AA2" s="90"/>
-      <c r="AB2" s="90"/>
-      <c r="AC2" s="90"/>
-      <c r="AD2" s="90"/>
-      <c r="AE2" s="90"/>
-      <c r="AF2" s="90"/>
-      <c r="AG2" s="91"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="X2" s="102"/>
+      <c r="Y2" s="102"/>
+      <c r="Z2" s="102"/>
+      <c r="AA2" s="102"/>
+      <c r="AB2" s="102"/>
+      <c r="AC2" s="102"/>
+      <c r="AD2" s="102"/>
+      <c r="AE2" s="102"/>
+      <c r="AF2" s="102"/>
+      <c r="AG2" s="103"/>
+      <c r="AH2" s="14"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
       <c r="L3" s="15"/>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
@@ -3686,25 +3669,26 @@
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
       <c r="R3" s="15"/>
-      <c r="S3" s="83" t="s">
+      <c r="S3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="83"/>
-      <c r="AB3" s="83"/>
-      <c r="AC3" s="83"/>
-      <c r="AD3" s="83"/>
-      <c r="AE3" s="83"/>
-      <c r="AF3" s="83"/>
-      <c r="AG3" s="84"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="T3" s="89"/>
+      <c r="U3" s="89"/>
+      <c r="V3" s="89"/>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="89"/>
+      <c r="AA3" s="89"/>
+      <c r="AB3" s="89"/>
+      <c r="AC3" s="89"/>
+      <c r="AD3" s="89"/>
+      <c r="AE3" s="89"/>
+      <c r="AF3" s="89"/>
+      <c r="AG3" s="90"/>
+      <c r="AH3" s="14"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="24"/>
       <c r="C4" s="15"/>
@@ -3717,242 +3701,248 @@
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="85" t="s">
+      <c r="M4" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88"/>
       <c r="R4" s="15"/>
-      <c r="S4" s="83" t="s">
+      <c r="S4" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="83"/>
-      <c r="W4" s="83"/>
-      <c r="X4" s="83"/>
-      <c r="Y4" s="83"/>
-      <c r="Z4" s="83"/>
-      <c r="AA4" s="83"/>
-      <c r="AB4" s="83"/>
-      <c r="AC4" s="83"/>
-      <c r="AD4" s="83"/>
-      <c r="AE4" s="83"/>
-      <c r="AF4" s="83"/>
-      <c r="AG4" s="84"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="89"/>
+      <c r="AD4" s="89"/>
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="14"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="95"/>
+      <c r="G5" s="97"/>
       <c r="H5" s="38"/>
       <c r="I5" s="15"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="85" t="s">
+      <c r="M5" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="88"/>
       <c r="R5" s="15"/>
-      <c r="S5" s="83" t="s">
+      <c r="S5" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="83"/>
-      <c r="U5" s="83"/>
-      <c r="V5" s="83"/>
-      <c r="W5" s="83"/>
-      <c r="X5" s="83"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="83"/>
-      <c r="AA5" s="83"/>
-      <c r="AB5" s="83"/>
-      <c r="AC5" s="83"/>
-      <c r="AD5" s="83"/>
-      <c r="AE5" s="83"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="84"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="T5" s="89"/>
+      <c r="U5" s="89"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="89"/>
+      <c r="X5" s="89"/>
+      <c r="Y5" s="89"/>
+      <c r="Z5" s="89"/>
+      <c r="AA5" s="89"/>
+      <c r="AB5" s="89"/>
+      <c r="AC5" s="89"/>
+      <c r="AD5" s="89"/>
+      <c r="AE5" s="89"/>
+      <c r="AF5" s="89"/>
+      <c r="AG5" s="90"/>
+      <c r="AH5" s="14"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="24"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
-      <c r="F6" s="77" t="s">
+      <c r="F6" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="77"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="38"/>
       <c r="I6" s="15"/>
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="85" t="s">
+      <c r="M6" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="85"/>
-      <c r="O6" s="85"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="88"/>
+      <c r="Q6" s="88"/>
       <c r="R6" s="15"/>
-      <c r="S6" s="83" t="s">
+      <c r="S6" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="83"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="83"/>
-      <c r="Z6" s="83"/>
-      <c r="AA6" s="83"/>
-      <c r="AB6" s="83"/>
-      <c r="AC6" s="83"/>
-      <c r="AD6" s="83"/>
-      <c r="AE6" s="83"/>
-      <c r="AF6" s="83"/>
-      <c r="AG6" s="84"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="T6" s="89"/>
+      <c r="U6" s="89"/>
+      <c r="V6" s="89"/>
+      <c r="W6" s="89"/>
+      <c r="X6" s="89"/>
+      <c r="Y6" s="89"/>
+      <c r="Z6" s="89"/>
+      <c r="AA6" s="89"/>
+      <c r="AB6" s="89"/>
+      <c r="AC6" s="89"/>
+      <c r="AD6" s="89"/>
+      <c r="AE6" s="89"/>
+      <c r="AF6" s="89"/>
+      <c r="AG6" s="90"/>
+      <c r="AH6" s="14"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="77" t="s">
+      <c r="F7" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="77"/>
+      <c r="G7" s="86"/>
       <c r="H7" s="38"/>
       <c r="I7" s="15"/>
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="85" t="s">
+      <c r="M7" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88"/>
       <c r="R7" s="15"/>
-      <c r="S7" s="83" t="s">
+      <c r="S7" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="T7" s="83"/>
-      <c r="U7" s="83"/>
-      <c r="V7" s="83"/>
-      <c r="W7" s="83"/>
-      <c r="X7" s="83"/>
-      <c r="Y7" s="83"/>
-      <c r="Z7" s="83"/>
-      <c r="AA7" s="83"/>
-      <c r="AB7" s="83"/>
-      <c r="AC7" s="83"/>
-      <c r="AD7" s="83"/>
-      <c r="AE7" s="83"/>
-      <c r="AF7" s="83"/>
-      <c r="AG7" s="84"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="T7" s="89"/>
+      <c r="U7" s="89"/>
+      <c r="V7" s="89"/>
+      <c r="W7" s="89"/>
+      <c r="X7" s="89"/>
+      <c r="Y7" s="89"/>
+      <c r="Z7" s="89"/>
+      <c r="AA7" s="89"/>
+      <c r="AB7" s="89"/>
+      <c r="AC7" s="89"/>
+      <c r="AD7" s="89"/>
+      <c r="AE7" s="89"/>
+      <c r="AF7" s="89"/>
+      <c r="AG7" s="90"/>
+      <c r="AH7" s="14"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="24"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="77" t="s">
+      <c r="F8" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="77"/>
+      <c r="G8" s="86"/>
       <c r="H8" s="38"/>
       <c r="I8" s="15"/>
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="85" t="s">
+      <c r="M8" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="85"/>
-      <c r="O8" s="85"/>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="82"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88"/>
       <c r="R8" s="15"/>
-      <c r="S8" s="83" t="s">
+      <c r="S8" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="T8" s="83"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="83"/>
-      <c r="Y8" s="83"/>
-      <c r="Z8" s="83"/>
-      <c r="AA8" s="83"/>
-      <c r="AB8" s="83"/>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="83"/>
-      <c r="AE8" s="83"/>
-      <c r="AF8" s="83"/>
-      <c r="AG8" s="84"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="T8" s="89"/>
+      <c r="U8" s="89"/>
+      <c r="V8" s="89"/>
+      <c r="W8" s="89"/>
+      <c r="X8" s="89"/>
+      <c r="Y8" s="89"/>
+      <c r="Z8" s="89"/>
+      <c r="AA8" s="89"/>
+      <c r="AB8" s="89"/>
+      <c r="AC8" s="89"/>
+      <c r="AD8" s="89"/>
+      <c r="AE8" s="89"/>
+      <c r="AF8" s="89"/>
+      <c r="AG8" s="90"/>
+      <c r="AH8" s="14"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="94"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="77" t="s">
+      <c r="F9" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="77"/>
+      <c r="G9" s="86"/>
       <c r="H9" s="38"/>
       <c r="I9" s="15"/>
       <c r="J9" s="39"/>
       <c r="K9" s="39"/>
       <c r="L9" s="15"/>
-      <c r="M9" s="85" t="s">
+      <c r="M9" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="82"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="88"/>
       <c r="R9" s="15"/>
-      <c r="S9" s="83" t="s">
+      <c r="S9" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="T9" s="83"/>
-      <c r="U9" s="83"/>
-      <c r="V9" s="83"/>
-      <c r="W9" s="83"/>
-      <c r="X9" s="83"/>
-      <c r="Y9" s="83"/>
-      <c r="Z9" s="83"/>
-      <c r="AA9" s="83"/>
-      <c r="AB9" s="83"/>
-      <c r="AC9" s="83"/>
-      <c r="AD9" s="83"/>
-      <c r="AE9" s="83"/>
-      <c r="AF9" s="83"/>
-      <c r="AG9" s="84"/>
-    </row>
-    <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T9" s="89"/>
+      <c r="U9" s="89"/>
+      <c r="V9" s="89"/>
+      <c r="W9" s="89"/>
+      <c r="X9" s="89"/>
+      <c r="Y9" s="89"/>
+      <c r="Z9" s="89"/>
+      <c r="AA9" s="89"/>
+      <c r="AB9" s="89"/>
+      <c r="AC9" s="89"/>
+      <c r="AD9" s="89"/>
+      <c r="AE9" s="89"/>
+      <c r="AF9" s="89"/>
+      <c r="AG9" s="90"/>
+      <c r="AH9" s="14"/>
+    </row>
+    <row r="10" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="25"/>
       <c r="C10" s="26"/>
@@ -3971,25 +3961,27 @@
       <c r="P10" s="26"/>
       <c r="Q10" s="26"/>
       <c r="R10" s="26"/>
-      <c r="S10" s="78" t="s">
+      <c r="S10" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="T10" s="78"/>
-      <c r="U10" s="78"/>
-      <c r="V10" s="78"/>
-      <c r="W10" s="78"/>
-      <c r="X10" s="78"/>
-      <c r="Y10" s="78"/>
-      <c r="Z10" s="78"/>
-      <c r="AA10" s="78"/>
-      <c r="AB10" s="78"/>
-      <c r="AC10" s="78"/>
-      <c r="AD10" s="78"/>
-      <c r="AE10" s="78"/>
-      <c r="AF10" s="78"/>
-      <c r="AG10" s="79"/>
-    </row>
-    <row r="11" spans="1:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T10" s="91"/>
+      <c r="U10" s="91"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="91"/>
+      <c r="X10" s="91"/>
+      <c r="Y10" s="91"/>
+      <c r="Z10" s="91"/>
+      <c r="AA10" s="91"/>
+      <c r="AB10" s="91"/>
+      <c r="AC10" s="91"/>
+      <c r="AD10" s="91"/>
+      <c r="AE10" s="91"/>
+      <c r="AF10" s="91"/>
+      <c r="AG10" s="92"/>
+      <c r="AH10" s="14"/>
+    </row>
+    <row r="11" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
       <c r="B11" s="27"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
@@ -4022,58 +4014,62 @@
       <c r="AE11" s="28"/>
       <c r="AF11" s="28"/>
       <c r="AG11" s="29"/>
-    </row>
-    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH11" s="14"/>
+    </row>
+    <row r="12" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
       <c r="B12" s="30"/>
-      <c r="C12" s="80" t="s">
+      <c r="C12" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="80" t="s">
+      <c r="G12" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="80" t="s">
+      <c r="K12" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="81"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="80" t="s">
+      <c r="O12" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="80"/>
-      <c r="Q12" s="80"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="81"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="80" t="s">
+      <c r="S12" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="T12" s="80"/>
-      <c r="U12" s="80"/>
+      <c r="T12" s="81"/>
+      <c r="U12" s="81"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="80" t="s">
+      <c r="W12" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="X12" s="80"/>
-      <c r="Y12" s="80"/>
+      <c r="X12" s="81"/>
+      <c r="Y12" s="81"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="80" t="s">
+      <c r="AA12" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="AB12" s="80"/>
-      <c r="AC12" s="80"/>
+      <c r="AB12" s="81"/>
+      <c r="AC12" s="81"/>
       <c r="AD12" s="1"/>
-      <c r="AE12" s="80" t="s">
+      <c r="AE12" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="AF12" s="80"/>
-      <c r="AG12" s="81"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AF12" s="81"/>
+      <c r="AG12" s="82"/>
+      <c r="AH12" s="14"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13" s="30"/>
       <c r="C13" s="19"/>
       <c r="D13" s="8"/>
@@ -4106,8 +4102,10 @@
       <c r="AE13" s="20"/>
       <c r="AF13" s="11"/>
       <c r="AG13" s="31"/>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH13" s="14"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
       <c r="B14" s="30"/>
       <c r="C14" s="20"/>
       <c r="D14" s="11"/>
@@ -4140,8 +4138,10 @@
       <c r="AE14" s="20"/>
       <c r="AF14" s="11"/>
       <c r="AG14" s="32"/>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH14" s="14"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
       <c r="B15" s="30"/>
       <c r="C15" s="20"/>
       <c r="D15" s="11"/>
@@ -4174,8 +4174,10 @@
       <c r="AE15" s="20"/>
       <c r="AF15" s="11"/>
       <c r="AG15" s="32"/>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH15" s="14"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
       <c r="B16" s="30"/>
       <c r="C16" s="20"/>
       <c r="D16" s="11"/>
@@ -4208,8 +4210,10 @@
       <c r="AE16" s="20"/>
       <c r="AF16" s="11"/>
       <c r="AG16" s="32"/>
-    </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH16" s="14"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
       <c r="B17" s="30"/>
       <c r="C17" s="20"/>
       <c r="D17" s="11"/>
@@ -4242,8 +4246,10 @@
       <c r="AE17" s="20"/>
       <c r="AF17" s="11"/>
       <c r="AG17" s="32"/>
-    </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH17" s="14"/>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
       <c r="B18" s="30"/>
       <c r="C18" s="20"/>
       <c r="D18" s="11"/>
@@ -4276,8 +4282,10 @@
       <c r="AE18" s="20"/>
       <c r="AF18" s="11"/>
       <c r="AG18" s="32"/>
-    </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH18" s="14"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
       <c r="B19" s="30"/>
       <c r="C19" s="20"/>
       <c r="D19" s="11"/>
@@ -4310,8 +4318,10 @@
       <c r="AE19" s="20"/>
       <c r="AF19" s="11"/>
       <c r="AG19" s="32"/>
-    </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH19" s="14"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
       <c r="B20" s="30"/>
       <c r="C20" s="20"/>
       <c r="D20" s="11"/>
@@ -4344,8 +4354,10 @@
       <c r="AE20" s="20"/>
       <c r="AF20" s="11"/>
       <c r="AG20" s="32"/>
-    </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH20" s="14"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
       <c r="B21" s="30"/>
       <c r="C21" s="20"/>
       <c r="D21" s="11"/>
@@ -4378,8 +4390,10 @@
       <c r="AE21" s="20"/>
       <c r="AF21" s="11"/>
       <c r="AG21" s="32"/>
-    </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH21" s="14"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
       <c r="B22" s="30"/>
       <c r="C22" s="20"/>
       <c r="D22" s="11"/>
@@ -4412,8 +4426,10 @@
       <c r="AE22" s="20"/>
       <c r="AF22" s="11"/>
       <c r="AG22" s="32"/>
-    </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH22" s="14"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
       <c r="B23" s="30"/>
       <c r="C23" s="20"/>
       <c r="D23" s="11"/>
@@ -4446,8 +4462,10 @@
       <c r="AE23" s="20"/>
       <c r="AF23" s="11"/>
       <c r="AG23" s="32"/>
-    </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH23" s="14"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
       <c r="B24" s="30"/>
       <c r="C24" s="20"/>
       <c r="D24" s="11"/>
@@ -4480,8 +4498,10 @@
       <c r="AE24" s="20"/>
       <c r="AF24" s="11"/>
       <c r="AG24" s="32"/>
-    </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH24" s="14"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
       <c r="B25" s="30"/>
       <c r="C25" s="20"/>
       <c r="D25" s="11"/>
@@ -4514,8 +4534,10 @@
       <c r="AE25" s="20"/>
       <c r="AF25" s="11"/>
       <c r="AG25" s="32"/>
-    </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH25" s="14"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
       <c r="B26" s="30"/>
       <c r="C26" s="20"/>
       <c r="D26" s="11"/>
@@ -4548,8 +4570,10 @@
       <c r="AE26" s="20"/>
       <c r="AF26" s="11"/>
       <c r="AG26" s="32"/>
-    </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH26" s="14"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
       <c r="B27" s="30"/>
       <c r="C27" s="20"/>
       <c r="D27" s="11"/>
@@ -4582,8 +4606,10 @@
       <c r="AE27" s="20"/>
       <c r="AF27" s="11"/>
       <c r="AG27" s="32"/>
-    </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH27" s="14"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
       <c r="B28" s="30"/>
       <c r="C28" s="20"/>
       <c r="D28" s="11"/>
@@ -4616,8 +4642,10 @@
       <c r="AE28" s="20"/>
       <c r="AF28" s="11"/>
       <c r="AG28" s="32"/>
-    </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH28" s="14"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
       <c r="B29" s="30"/>
       <c r="C29" s="20"/>
       <c r="D29" s="11"/>
@@ -4650,8 +4678,10 @@
       <c r="AE29" s="20"/>
       <c r="AF29" s="11"/>
       <c r="AG29" s="32"/>
-    </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH29" s="14"/>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
       <c r="B30" s="30"/>
       <c r="C30" s="20"/>
       <c r="D30" s="11"/>
@@ -4684,8 +4714,10 @@
       <c r="AE30" s="20"/>
       <c r="AF30" s="11"/>
       <c r="AG30" s="32"/>
-    </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH30" s="14"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
       <c r="B31" s="30"/>
       <c r="C31" s="20"/>
       <c r="D31" s="11"/>
@@ -4718,8 +4750,10 @@
       <c r="AE31" s="20"/>
       <c r="AF31" s="11"/>
       <c r="AG31" s="32"/>
-    </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH31" s="14"/>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32" s="30"/>
       <c r="C32" s="20"/>
       <c r="D32" s="11"/>
@@ -4752,8 +4786,10 @@
       <c r="AE32" s="20"/>
       <c r="AF32" s="11"/>
       <c r="AG32" s="32"/>
-    </row>
-    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH32" s="14"/>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
       <c r="B33" s="30"/>
       <c r="C33" s="20"/>
       <c r="D33" s="11"/>
@@ -4786,8 +4822,10 @@
       <c r="AE33" s="20"/>
       <c r="AF33" s="11"/>
       <c r="AG33" s="32"/>
-    </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH33" s="14"/>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
       <c r="B34" s="30"/>
       <c r="C34" s="20"/>
       <c r="D34" s="11"/>
@@ -4820,8 +4858,10 @@
       <c r="AE34" s="20"/>
       <c r="AF34" s="11"/>
       <c r="AG34" s="32"/>
-    </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH34" s="14"/>
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
       <c r="B35" s="30"/>
       <c r="C35" s="20"/>
       <c r="D35" s="11"/>
@@ -4854,8 +4894,10 @@
       <c r="AE35" s="20"/>
       <c r="AF35" s="11"/>
       <c r="AG35" s="32"/>
-    </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH35" s="14"/>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
       <c r="B36" s="30"/>
       <c r="C36" s="20"/>
       <c r="D36" s="11"/>
@@ -4888,8 +4930,10 @@
       <c r="AE36" s="20"/>
       <c r="AF36" s="11"/>
       <c r="AG36" s="32"/>
-    </row>
-    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH36" s="14"/>
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
       <c r="B37" s="30"/>
       <c r="C37" s="20"/>
       <c r="D37" s="11"/>
@@ -4922,8 +4966,10 @@
       <c r="AE37" s="20"/>
       <c r="AF37" s="11"/>
       <c r="AG37" s="32"/>
-    </row>
-    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH37" s="14"/>
+    </row>
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
       <c r="B38" s="30"/>
       <c r="C38" s="20"/>
       <c r="D38" s="11"/>
@@ -4956,8 +5002,10 @@
       <c r="AE38" s="20"/>
       <c r="AF38" s="11"/>
       <c r="AG38" s="32"/>
-    </row>
-    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH38" s="14"/>
+    </row>
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
       <c r="B39" s="30"/>
       <c r="C39" s="20"/>
       <c r="D39" s="11"/>
@@ -4990,8 +5038,10 @@
       <c r="AE39" s="20"/>
       <c r="AF39" s="11"/>
       <c r="AG39" s="32"/>
-    </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH39" s="14"/>
+    </row>
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
       <c r="B40" s="30"/>
       <c r="C40" s="20"/>
       <c r="D40" s="11"/>
@@ -5024,8 +5074,10 @@
       <c r="AE40" s="20"/>
       <c r="AF40" s="11"/>
       <c r="AG40" s="32"/>
-    </row>
-    <row r="41" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH40" s="14"/>
+    </row>
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
       <c r="B41" s="30"/>
       <c r="C41" s="20"/>
       <c r="D41" s="11"/>
@@ -5058,8 +5110,10 @@
       <c r="AE41" s="20"/>
       <c r="AF41" s="11"/>
       <c r="AG41" s="32"/>
-    </row>
-    <row r="42" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH41" s="14"/>
+    </row>
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
       <c r="B42" s="30"/>
       <c r="C42" s="20"/>
       <c r="D42" s="11"/>
@@ -5092,8 +5146,10 @@
       <c r="AE42" s="20"/>
       <c r="AF42" s="11"/>
       <c r="AG42" s="32"/>
-    </row>
-    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH42" s="14"/>
+    </row>
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
       <c r="B43" s="30"/>
       <c r="C43" s="20"/>
       <c r="D43" s="11"/>
@@ -5126,8 +5182,10 @@
       <c r="AE43" s="20"/>
       <c r="AF43" s="11"/>
       <c r="AG43" s="32"/>
-    </row>
-    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH43" s="14"/>
+    </row>
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
       <c r="B44" s="30"/>
       <c r="C44" s="20"/>
       <c r="D44" s="11"/>
@@ -5160,8 +5218,10 @@
       <c r="AE44" s="20"/>
       <c r="AF44" s="11"/>
       <c r="AG44" s="32"/>
-    </row>
-    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH44" s="14"/>
+    </row>
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
       <c r="B45" s="30"/>
       <c r="C45" s="20"/>
       <c r="D45" s="11"/>
@@ -5194,8 +5254,10 @@
       <c r="AE45" s="20"/>
       <c r="AF45" s="11"/>
       <c r="AG45" s="32"/>
-    </row>
-    <row r="46" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH45" s="14"/>
+    </row>
+    <row r="46" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="14"/>
       <c r="B46" s="33"/>
       <c r="C46" s="34"/>
       <c r="D46" s="35"/>
@@ -5228,51 +5290,86 @@
       <c r="AE46" s="34"/>
       <c r="AF46" s="35"/>
       <c r="AG46" s="37"/>
-    </row>
-    <row r="47" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="AH46" s="14"/>
+    </row>
+    <row r="47" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="14"/>
+      <c r="W47" s="14"/>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="14"/>
+      <c r="Z47" s="14"/>
+      <c r="AA47" s="14"/>
+      <c r="AB47" s="14"/>
+      <c r="AC47" s="14"/>
+      <c r="AD47" s="14"/>
+      <c r="AE47" s="14"/>
+      <c r="AF47" s="14"/>
+      <c r="AG47" s="14"/>
+      <c r="AH47" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="S5:AG5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="M6:O6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:Q5"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="S6:AG6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="S7:AG7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="M8:O8"/>
     <mergeCell ref="B2:K3"/>
     <mergeCell ref="S2:AG2"/>
     <mergeCell ref="S3:AG3"/>
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="S4:AG4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="S5:AG5"/>
+    <mergeCell ref="S10:AG10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S7:AG7"/>
     <mergeCell ref="F8:G8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="S8:AG8"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="S10:AG10"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="S9:AG9"/>
+    <mergeCell ref="AA12:AC12"/>
+    <mergeCell ref="AE12:AG12"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="O12:Q12"/>
     <mergeCell ref="S12:U12"/>
     <mergeCell ref="W12:Y12"/>
-    <mergeCell ref="AA12:AC12"/>
-    <mergeCell ref="AE12:AG12"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="S8:AG8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="S9:AG9"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5281,7 +5378,7 @@
   <dimension ref="B2:S13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5290,46 +5387,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="114"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="118"/>
     </row>
     <row r="3" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="116"/>
-      <c r="R3" s="116"/>
-      <c r="S3" s="117"/>
+      <c r="B3" s="119"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="121"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="15"/>
@@ -5352,28 +5449,28 @@
       <c r="S4" s="43"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="122"/>
-      <c r="D5" s="122"/>
-      <c r="E5" s="123"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="127"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="118" t="s">
+      <c r="G5" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="119"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="132"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="135"/>
+      <c r="K5" s="136"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="126" t="s">
+      <c r="M5" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="126"/>
-      <c r="O5" s="126"/>
-      <c r="P5" s="124"/>
-      <c r="Q5" s="125"/>
+      <c r="N5" s="130"/>
+      <c r="O5" s="130"/>
+      <c r="P5" s="128"/>
+      <c r="Q5" s="129"/>
       <c r="R5" s="43"/>
       <c r="S5" s="43"/>
     </row>
@@ -5383,45 +5480,47 @@
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="118" t="s">
+      <c r="G6" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="119"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="125"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="129"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="126" t="s">
+      <c r="M6" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="126"/>
-      <c r="O6" s="126"/>
-      <c r="P6" s="131"/>
-      <c r="Q6" s="132"/>
+      <c r="N6" s="130"/>
+      <c r="O6" s="130"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="136"/>
       <c r="R6" s="43"/>
       <c r="S6" s="43"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="121"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="123"/>
+      <c r="B7" s="125" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="127"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="118" t="s">
+      <c r="G7" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="119"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="133"/>
-      <c r="K7" s="94"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="85"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="126" t="s">
+      <c r="M7" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="126"/>
-      <c r="O7" s="126"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="132"/>
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="136"/>
       <c r="R7" s="43"/>
       <c r="S7" s="43"/>
     </row>
@@ -5431,45 +5530,45 @@
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="118" t="s">
+      <c r="G8" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="119"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="132"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="135"/>
+      <c r="K8" s="136"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="126" t="s">
+      <c r="M8" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="126"/>
-      <c r="O8" s="126"/>
-      <c r="P8" s="124"/>
-      <c r="Q8" s="125"/>
+      <c r="N8" s="130"/>
+      <c r="O8" s="130"/>
+      <c r="P8" s="128"/>
+      <c r="Q8" s="129"/>
       <c r="R8" s="43"/>
       <c r="S8" s="43"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="121"/>
-      <c r="C9" s="122"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="123"/>
+      <c r="B9" s="125"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="127"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="118" t="s">
+      <c r="G9" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="119"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="131"/>
-      <c r="K9" s="132"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="135"/>
+      <c r="K9" s="136"/>
       <c r="L9" s="15"/>
-      <c r="M9" s="126" t="s">
+      <c r="M9" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="126"/>
-      <c r="O9" s="126"/>
-      <c r="P9" s="133"/>
-      <c r="Q9" s="94"/>
+      <c r="N9" s="130"/>
+      <c r="O9" s="130"/>
+      <c r="P9" s="137"/>
+      <c r="Q9" s="85"/>
       <c r="R9" s="43"/>
       <c r="S9" s="43"/>
     </row>
@@ -5495,50 +5594,50 @@
     </row>
     <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:19" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="106" t="s">
+      <c r="C12" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="106" t="s">
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="107"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="106" t="s">
+      <c r="H12" s="111"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="107"/>
-      <c r="L12" s="108"/>
-      <c r="M12" s="103" t="s">
+      <c r="K12" s="111"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="104"/>
-      <c r="O12" s="105"/>
-      <c r="P12" s="103" t="s">
+      <c r="N12" s="108"/>
+      <c r="O12" s="109"/>
+      <c r="P12" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="Q12" s="104"/>
-      <c r="R12" s="105"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="109"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C13" s="127"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="109"/>
-      <c r="K13" s="110"/>
-      <c r="L13" s="111"/>
-      <c r="M13" s="128"/>
-      <c r="N13" s="129"/>
-      <c r="O13" s="130"/>
-      <c r="P13" s="100"/>
-      <c r="Q13" s="101"/>
-      <c r="R13" s="102"/>
+      <c r="C13" s="131"/>
+      <c r="D13" s="114"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="115"/>
+      <c r="M13" s="132"/>
+      <c r="N13" s="133"/>
+      <c r="O13" s="134"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="105"/>
+      <c r="R13" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="34">

</xml_diff>